<commit_message>
changes made to SMTP activity
</commit_message>
<xml_diff>
--- a/Output/Result.xlsx
+++ b/Output/Result.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <x:si>
     <x:t>Book Name</x:t>
   </x:si>
@@ -33,45 +33,81 @@
     <x:t xml:space="preserve"> Vaibhav Srivastava </x:t>
   </x:si>
   <x:si>
+    <x:t>₹570.13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Learning Robotic Process Automation: Create Software robots and automate business processes with the leading RPA tool – UiPath</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Alok Mani Tripathi  </x:t>
+  </x:si>
+  <x:si>
+    <x:t>₹2,971</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Robotic Process Automation Projects: Build real-world RPA solutions using UiPath and Automation Anywhere</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Nandan Mullakara and Arun Kumar Asokan  </x:t>
+  </x:si>
+  <x:si>
+    <x:t>₹390.58</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPA for everyone: Robotic Process Automation, this famous unknown</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Vincenzo Marchica </x:t>
+  </x:si>
+  <x:si>
+    <x:t>₹0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Real World RPA Use Cases for Businesses : To Save Money And Increase Productivity</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Srikanth Merianda </x:t>
+  </x:si>
+  <x:si>
+    <x:t>₹209</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Introduction To RPA</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Abhinav Sabharwal  </x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPA Tutorial: A Guide To Learning Rpa For The Average Worker To Preserve Your Job</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Terrell Tromburg </x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPA (Japanese Edition)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Author not Available</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RPA for Developers : Automation Solutions Every Developer Should Know</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> Stijn Van Hijfte </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Robotic Process Automation (RPA): Business Presentation (FlevyPro Frameworks)</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve"> FlevyPro Library </x:t>
+  </x:si>
+  <x:si>
     <x:t>₹645.63</x:t>
   </x:si>
   <x:si>
-    <x:t>Robotic Process Automation Projects: Build real-world RPA solutions using UiPath and Automation Anywhere</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Nandan Mullakara and Arun Kumar Asokan  </x:t>
-  </x:si>
-  <x:si>
-    <x:t>₹390.58</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RPA for everyone: Robotic Process Automation, this famous unknown</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Vincenzo Marchica </x:t>
-  </x:si>
-  <x:si>
-    <x:t>₹0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Learning Robotic Process Automation: Create Software robots and automate business processes with the leading RPA tool – UiPath</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Alok Mani Tripathi  </x:t>
-  </x:si>
-  <x:si>
     <x:t>₹2,974</x:t>
   </x:si>
   <x:si>
-    <x:t>Real World RPA Use Cases for Businesses : To Save Money And Increase Productivity</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Srikanth Merianda </x:t>
-  </x:si>
-  <x:si>
-    <x:t>₹209</x:t>
-  </x:si>
-  <x:si>
     <x:t>RPA in Oracle</x:t>
   </x:si>
   <x:si>
@@ -79,24 +115,6 @@
   </x:si>
   <x:si>
     <x:t>₹405</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Introduction To RPA</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Abhinav Sabharwal  </x:t>
-  </x:si>
-  <x:si>
-    <x:t>RPA Tutorial: A Guide To Learning Rpa For The Average Worker To Preserve Your Job</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve"> Terrell Tromburg </x:t>
-  </x:si>
-  <x:si>
-    <x:t>RPA (Japanese Edition)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Author not Available</x:t>
   </x:si>
   <x:si>
     <x:t>RPA robotic process automation Second Edition</x:t>
@@ -159,8 +177,20 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="8">
+  <x:cellStyleXfs count="12">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -595,50 +625,50 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="C7" s="4" t="s">
-        <x:v>20</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3">
       <x:c r="A8" s="6" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B8" s="4" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="B8" s="4" t="s">
-        <x:v>22</x:v>
-      </x:c>
       <x:c r="C8" s="4" t="s">
-        <x:v>11</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
       <x:c r="A9" s="6" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B9" s="4" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="B9" s="4" t="s">
-        <x:v>24</x:v>
-      </x:c>
       <x:c r="C9" s="4" t="s">
-        <x:v>11</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
       <x:c r="A10" s="6" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B10" s="4" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="B10" s="4" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="C10" s="4" t="s">
-        <x:v>11</x:v>
-      </x:c>
+      <x:c r="C10" s="4" t="s"/>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="A11" s="6" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B11" s="4" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="B11" s="4" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="C11" s="4" t="s"/>
+      <x:c r="C11" s="4" t="s">
+        <x:v>14</x:v>
+      </x:c>
     </x:row>
     <x:row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="C12" s="4" t="s"/>
@@ -695,40 +725,40 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C2" s="4" t="s">
-        <x:v>5</x:v>
+        <x:v>28</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A3" s="4" t="s">
-        <x:v>6</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B3" s="4" t="s">
-        <x:v>7</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C3" s="4" t="s">
-        <x:v>8</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A4" s="4" t="s">
-        <x:v>9</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B4" s="4" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C4" s="4" t="s">
-        <x:v>11</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A5" s="4" t="s">
-        <x:v>12</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B5" s="4" t="s">
-        <x:v>13</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C5" s="4" t="s">
-        <x:v>14</x:v>
+        <x:v>29</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -744,54 +774,54 @@
     </x:row>
     <x:row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A7" s="4" t="s">
-        <x:v>18</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B7" s="4" t="s">
-        <x:v>19</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C7" s="4" t="s">
-        <x:v>20</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A8" s="4" t="s">
-        <x:v>21</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B8" s="4" t="s">
-        <x:v>22</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="C8" s="4" t="s">
-        <x:v>11</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A9" s="4" t="s">
-        <x:v>23</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B9" s="4" t="s">
-        <x:v>24</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="C9" s="4" t="s">
-        <x:v>11</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A10" s="4" t="s">
-        <x:v>25</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B10" s="4" t="s">
-        <x:v>26</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="C10" s="4" t="s">
-        <x:v>11</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A11" s="4" t="s">
-        <x:v>27</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B11" s="4" t="s">
-        <x:v>28</x:v>
+        <x:v>34</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>